<commit_message>
table1 is filling up correctly
</commit_message>
<xml_diff>
--- a/Analyse_NP.xlsx
+++ b/Analyse_NP.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GAYRARD\Documents\GitHub\Planetary-Nebula-Analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097410E6-16C6-4550-BE8B-AE4B07314491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="795" windowWidth="22860" windowHeight="9120"/>
+    <workbookView xWindow="4404" yWindow="720" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,17 +25,30 @@
     <definedName name="RO">Feuil1!$J$15</definedName>
     <definedName name="ROIII">Feuil1!$I$15</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>FM</author>
   </authors>
   <commentList>
-    <comment ref="I13" authorId="0">
+    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -45,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K13" authorId="0">
+    <comment ref="K13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M13" authorId="0">
+    <comment ref="M13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -85,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K21" authorId="0">
+    <comment ref="K21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -111,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O31" authorId="0">
+    <comment ref="O31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -753,7 +772,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -1279,7 +1298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1385,9 +1404,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1405,11 +1421,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1417,9 +1430,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1459,15 +1469,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1508,7 +1516,6 @@
     <xf numFmtId="1" fontId="0" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1566,12 +1573,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -1602,11 +1612,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E5FB-4C10-9AB7-16B34969D34C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1657,7 +1672,7 @@
             <a:pPr>
               <a:defRPr sz="800"/>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="146456576"/>
@@ -1684,7 +1699,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -1715,11 +1730,16 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0470-4CF5-B537-8383F40F86B6}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1769,7 +1789,7 @@
             <a:pPr>
               <a:defRPr sz="800"/>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="146360576"/>
@@ -1796,7 +1816,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -1827,11 +1847,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>7.9662956114738126</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F869-4F99-A551-660FF9BF5A14}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1881,7 +1906,7 @@
             <a:pPr>
               <a:defRPr sz="800"/>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="146372096"/>
@@ -1908,7 +1933,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -2800,6 +2825,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0492-4E4A-BC22-2598A119C586}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2857,7 +2887,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="146715008"/>
@@ -2911,7 +2941,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="146709120"/>
@@ -2971,7 +3001,7 @@
           <a:latin typeface="Calibri"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2983,7 +3013,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -3875,6 +3905,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4B5A-49B0-AE96-2DFFB5B58889}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3932,7 +3967,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="146547840"/>
@@ -3986,7 +4021,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="146726272"/>
@@ -4046,7 +4081,7 @@
           <a:latin typeface="Calibri"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4058,7 +4093,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -4404,6 +4439,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A72D-450D-A49E-BFE0BF2B9F5F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4739,6 +4779,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A72D-450D-A49E-BFE0BF2B9F5F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -5074,6 +5119,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A72D-450D-A49E-BFE0BF2B9F5F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -5409,6 +5459,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A72D-450D-A49E-BFE0BF2B9F5F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5464,7 +5519,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="146596224"/>
@@ -5516,7 +5571,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="146590336"/>
@@ -5574,7 +5629,7 @@
           <a:latin typeface="Calibri"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5602,7 +5657,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5632,7 +5693,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Graphique 3"/>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5664,7 +5731,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Graphique 4"/>
+        <xdr:cNvPr id="5" name="Graphique 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5696,7 +5769,13 @@
     <xdr:ext cx="4572000" cy="2743200"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5721,7 +5800,13 @@
     <xdr:ext cx="4572000" cy="2743200"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5746,7 +5831,13 @@
     <xdr:ext cx="4572000" cy="2743200"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Graphique 4"/>
+        <xdr:cNvPr id="4" name="Graphique 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5765,9 +5856,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5805,7 +5896,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -5877,7 +5968,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6050,60 +6141,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:S35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.375" customWidth="1"/>
-    <col min="2" max="2" width="8.125" customWidth="1"/>
-    <col min="3" max="3" width="6.125" customWidth="1"/>
-    <col min="4" max="4" width="9.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.25" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="4.625" customWidth="1"/>
-    <col min="9" max="9" width="11.625" customWidth="1"/>
+    <col min="1" max="1" width="2.3984375" customWidth="1"/>
+    <col min="2" max="2" width="8.09765625" customWidth="1"/>
+    <col min="3" max="3" width="6.09765625" customWidth="1"/>
+    <col min="4" max="4" width="9.19921875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.59765625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="4.59765625" customWidth="1"/>
+    <col min="9" max="9" width="11.59765625" customWidth="1"/>
     <col min="10" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="12.25" customWidth="1"/>
+    <col min="13" max="13" width="12.19921875" customWidth="1"/>
     <col min="14" max="18" width="11" customWidth="1"/>
-    <col min="19" max="19" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:19" s="46" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="112" t="s">
+    <row r="1" spans="2:19" ht="4.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:19" s="45" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="106" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
-      <c r="P2" s="113"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="115" t="s">
+      <c r="C2" s="107"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="107"/>
+      <c r="J2" s="107"/>
+      <c r="K2" s="107"/>
+      <c r="L2" s="107"/>
+      <c r="M2" s="107"/>
+      <c r="N2" s="107"/>
+      <c r="O2" s="107"/>
+      <c r="P2" s="107"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="109" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="2:19" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <v>1</v>
       </c>
@@ -6130,7 +6221,7 @@
       <c r="L4" s="6"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="2:19" s="8" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" s="8" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
@@ -6164,39 +6255,39 @@
       <c r="M5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="43"/>
+      <c r="O5" s="3"/>
       <c r="Q5" s="18"/>
       <c r="R5" s="18"/>
       <c r="S5" s="18"/>
     </row>
-    <row r="6" spans="2:19" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="Q6" s="18"/>
       <c r="R6" s="18"/>
       <c r="S6" s="18"/>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" s="19">
         <v>4340.47</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="51" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="21">
-        <v>23.7</v>
+        <v>222.15</v>
       </c>
       <c r="E7" s="22">
         <f t="shared" ref="E7:E19" si="0">+D7/D$10*100</f>
-        <v>43.807763401109057</v>
+        <v>45.944324950363999</v>
       </c>
       <c r="F7" s="23">
         <f t="shared" ref="F7:F19" si="1">+E7*10^(J$11*((2.5634*(B7/10000)^2-4.873*(B7/10000)+1.7636)))</f>
-        <v>45.462450010559465</v>
+        <v>60.799645518314634</v>
       </c>
       <c r="G7" s="24">
         <f>-(E7-F7)/F7*100</f>
-        <v>3.6396776000107294</v>
+        <v>24.433235492262494</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="4">
@@ -6207,40 +6298,40 @@
       </c>
       <c r="K7" s="26">
         <f>+E16/100</f>
-        <v>3.0979667282809604</v>
+        <v>5.6477084712111187</v>
       </c>
       <c r="L7" s="27">
         <v>2.86</v>
       </c>
       <c r="M7" s="26">
         <f>+F16/F10</f>
-        <v>2.8218954987137805</v>
+        <v>2.7897979733144567</v>
       </c>
       <c r="Q7" s="18"/>
       <c r="R7" s="18"/>
       <c r="S7" s="28"/>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" s="19">
         <v>4363.21</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="50" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="21">
-        <v>7</v>
+        <v>218.02</v>
       </c>
       <c r="E8" s="22">
         <f t="shared" si="0"/>
-        <v>12.939001848428836</v>
+        <v>45.090172071475848</v>
       </c>
       <c r="F8" s="23">
         <f t="shared" si="1"/>
-        <v>13.404989914636737</v>
+        <v>58.910045440104589</v>
       </c>
       <c r="G8" s="24">
         <f t="shared" ref="G8:G19" si="2">+(E8-F8)/F8*100</f>
-        <v>-3.4762283983451145</v>
+        <v>-23.459281461053656</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="4">
@@ -6263,27 +6354,25 @@
       <c r="R8" s="18"/>
       <c r="S8" s="28"/>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B9" s="19">
         <v>4685.68</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="21">
-        <v>16.600000000000001</v>
-      </c>
+      <c r="D9" s="21"/>
       <c r="E9" s="22">
         <f t="shared" si="0"/>
-        <v>30.683918669131238</v>
+        <v>0</v>
       </c>
       <c r="F9" s="23">
         <f t="shared" si="1"/>
-        <v>31.059078971726535</v>
-      </c>
-      <c r="G9" s="24">
+        <v>0</v>
+      </c>
+      <c r="G9" s="24" t="e">
         <f t="shared" si="2"/>
-        <v>-1.2078925551424449</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="4">
@@ -6294,28 +6383,28 @@
       </c>
       <c r="K9" s="26">
         <f>+E7/100</f>
-        <v>0.43807763401109057</v>
+        <v>0.45944324950364002</v>
       </c>
       <c r="L9" s="27">
         <v>0.46899999999999997</v>
       </c>
       <c r="M9" s="26">
         <f>+F7/F10</f>
-        <v>0.4545642067744356</v>
+        <v>0.60738742894058606</v>
       </c>
       <c r="Q9" s="18"/>
       <c r="R9" s="18"/>
       <c r="S9" s="28"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B10" s="19">
         <v>4861.33</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="51" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="21">
-        <v>54.1</v>
+        <v>483.52</v>
       </c>
       <c r="E10" s="22">
         <f t="shared" si="0"/>
@@ -6323,11 +6412,11 @@
       </c>
       <c r="F10" s="23">
         <f t="shared" si="1"/>
-        <v>100.01326398565054</v>
+        <v>100.10026981355583</v>
       </c>
       <c r="G10" s="24">
         <f t="shared" si="2"/>
-        <v>-1.3262226550712582E-2</v>
+        <v>-0.10016937391136524</v>
       </c>
       <c r="H10" s="25"/>
       <c r="I10" s="29"/>
@@ -6336,27 +6425,27 @@
       <c r="R10" s="18"/>
       <c r="S10" s="28"/>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B11" s="19">
         <v>4958.92</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="50" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="21">
-        <v>179</v>
+        <v>476.57</v>
       </c>
       <c r="E11" s="22">
         <f t="shared" si="0"/>
-        <v>330.86876155268021</v>
+        <v>98.562624090006622</v>
       </c>
       <c r="F11" s="23">
         <f t="shared" si="1"/>
-        <v>328.7735197409848</v>
+        <v>93.943126182558984</v>
       </c>
       <c r="G11" s="24">
         <f t="shared" si="2"/>
-        <v>0.63729031868080344</v>
+        <v>4.9173346631775932</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="30" t="s">
@@ -6364,40 +6453,40 @@
       </c>
       <c r="J11" s="31">
         <f>3.08*LOG(E16)-7.55</f>
-        <v>0.1225163874980808</v>
+        <v>0.92576659405347161</v>
       </c>
       <c r="L11" s="30" t="s">
         <v>18</v>
       </c>
       <c r="M11" s="32">
         <f>+J11/1.46</f>
-        <v>8.391533390279507E-2</v>
+        <v>0.63408670825580249</v>
       </c>
       <c r="Q11" s="18"/>
       <c r="R11" s="18"/>
       <c r="S11" s="28"/>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B12" s="19">
         <v>5006.8500000000004</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="50" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="21">
-        <v>552.9</v>
+        <v>1446.62</v>
       </c>
       <c r="E12" s="22">
         <f t="shared" si="0"/>
-        <v>1021.9963031423289</v>
+        <v>299.18514228987425</v>
       </c>
       <c r="F12" s="23">
         <f t="shared" si="1"/>
-        <v>1012.346047861558</v>
+        <v>278.48748523886042</v>
       </c>
       <c r="G12" s="24">
         <f t="shared" si="2"/>
-        <v>0.95325657675611619</v>
+        <v>7.4321677447233681</v>
       </c>
       <c r="H12" s="25"/>
       <c r="I12" s="29"/>
@@ -6406,55 +6495,55 @@
       <c r="R12" s="18"/>
       <c r="S12" s="28"/>
     </row>
-    <row r="13" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19">
         <v>5754.57</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="48" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="21">
-        <v>0.8</v>
+        <v>3.96</v>
       </c>
       <c r="E13" s="22">
         <f t="shared" si="0"/>
-        <v>1.478743068391867</v>
+        <v>0.81899404367968243</v>
       </c>
       <c r="F13" s="23">
         <f t="shared" si="1"/>
-        <v>1.4008855059632634</v>
+        <v>0.54423117572891466</v>
       </c>
       <c r="G13" s="24">
         <f t="shared" si="2"/>
-        <v>5.5577391654907489</v>
+        <v>50.48642565960408</v>
       </c>
       <c r="H13" s="25"/>
-      <c r="I13" s="90" t="s">
+      <c r="I13" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="91">
+      <c r="J13" s="86">
         <f>+F12/F11</f>
-        <v>3.0791593211615917</v>
-      </c>
-      <c r="K13" s="90" t="s">
+        <v>2.9644264200626851</v>
+      </c>
+      <c r="K13" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="92">
+      <c r="L13" s="87">
         <f>+F17/F15</f>
-        <v>3.0283431313591747</v>
-      </c>
-      <c r="M13" s="90" t="s">
+        <v>0.1813467636846352</v>
+      </c>
+      <c r="M13" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="N13" s="93">
+      <c r="N13" s="88">
         <f>+F17/F16</f>
-        <v>0.27481985453282998</v>
+        <v>0.18357214483056364</v>
       </c>
       <c r="Q13" s="18"/>
       <c r="R13" s="18"/>
       <c r="S13" s="28"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B14" s="33">
         <v>5875.65</v>
       </c>
@@ -6462,19 +6551,19 @@
         <v>22</v>
       </c>
       <c r="D14" s="21">
-        <v>6</v>
+        <v>88.12</v>
       </c>
       <c r="E14" s="22">
         <f t="shared" si="0"/>
-        <v>11.090573012939002</v>
+        <v>18.224685638649902</v>
       </c>
       <c r="F14" s="23">
         <f t="shared" si="1"/>
-        <v>10.438970970086348</v>
+        <v>11.533422560523382</v>
       </c>
       <c r="G14" s="24">
         <f t="shared" si="2"/>
-        <v>6.2420141287859483</v>
+        <v>58.01628305052644</v>
       </c>
       <c r="H14" s="25"/>
       <c r="L14" s="34">
@@ -6496,27 +6585,27 @@
       <c r="R14" s="18"/>
       <c r="S14" s="28"/>
     </row>
-    <row r="15" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="19">
         <v>6548.06</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="48" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="21">
-        <v>15.2</v>
+        <v>2751.17</v>
       </c>
       <c r="E15" s="22">
         <f t="shared" si="0"/>
-        <v>28.096118299445472</v>
+        <v>568.98783917935145</v>
       </c>
       <c r="F15" s="23">
         <f t="shared" si="1"/>
-        <v>25.611885468091611</v>
+        <v>282.68643905241765</v>
       </c>
       <c r="G15" s="24">
         <f t="shared" si="2"/>
-        <v>9.6995312369674025</v>
+        <v>101.27878828805291</v>
       </c>
       <c r="H15" s="25"/>
       <c r="I15" s="4" t="s">
@@ -6524,56 +6613,56 @@
       </c>
       <c r="J15" s="22">
         <f>+(F12+F11)/E8</f>
-        <v>103.6493837247108</v>
+        <v>8.2596848561822167</v>
       </c>
       <c r="K15" s="36" t="s">
         <v>24</v>
       </c>
       <c r="L15" s="37">
         <f>3.29*10000/LN($J15/7.9)</f>
-        <v>12780.912344200062</v>
+        <v>738932.72504881828</v>
       </c>
       <c r="M15" s="37">
         <f>14320/(LOG(RO)-0.89)</f>
-        <v>12722.479877758115</v>
+        <v>531088.76893697469</v>
       </c>
       <c r="N15" s="37">
         <f>-32990/(LN(1/(RO*0.132)))</f>
-        <v>12610.564448625826</v>
+        <v>381682.58021789859</v>
       </c>
       <c r="O15" s="37">
         <f>3.29*10000/LN($J15/8.32)</f>
-        <v>13043.383603012593</v>
-      </c>
-      <c r="P15" s="45">
+        <v>-4521826.4512508111</v>
+      </c>
+      <c r="P15" s="44">
         <f>14516/(LOG(J15)-0.871411)</f>
-        <v>12687.084190274094</v>
-      </c>
-      <c r="Q15" s="75"/>
-      <c r="R15" s="116"/>
+        <v>318665.43467460235</v>
+      </c>
+      <c r="Q15" s="72"/>
+      <c r="R15" s="110"/>
       <c r="S15" s="28"/>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B16" s="19">
         <v>6562.82</v>
       </c>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="51" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="21">
-        <v>167.6</v>
+        <v>2730.78</v>
       </c>
       <c r="E16" s="22">
         <f t="shared" si="0"/>
-        <v>309.79667282809606</v>
+        <v>564.77084712111184</v>
       </c>
       <c r="F16" s="23">
         <f t="shared" si="1"/>
-        <v>282.22697945278031</v>
+        <v>279.25952985408833</v>
       </c>
       <c r="G16" s="24">
         <f t="shared" si="2"/>
-        <v>9.7686243281105121</v>
+        <v>102.23870154626475</v>
       </c>
       <c r="H16" s="25"/>
       <c r="I16" s="1"/>
@@ -6588,34 +6677,34 @@
       <c r="N16" s="39">
         <v>8</v>
       </c>
-      <c r="O16" s="70" t="s">
+      <c r="O16" s="67" t="s">
         <v>81</v>
       </c>
       <c r="Q16" s="18"/>
       <c r="R16" s="18"/>
       <c r="S16" s="28"/>
     </row>
-    <row r="17" spans="2:19" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:19" ht="18" x14ac:dyDescent="0.4">
       <c r="B17" s="19">
         <v>6583.39</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="48" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="21">
-        <v>46.1</v>
+        <v>504.61</v>
       </c>
       <c r="E17" s="22">
         <f t="shared" si="0"/>
-        <v>85.212569316081328</v>
+        <v>104.3617637326274</v>
       </c>
       <c r="F17" s="23">
         <f t="shared" si="1"/>
-        <v>77.561577438453085</v>
+        <v>51.264270859689816</v>
       </c>
       <c r="G17" s="24">
         <f t="shared" si="2"/>
-        <v>9.8644098409415193</v>
+        <v>103.57602279814979</v>
       </c>
       <c r="H17" s="25"/>
       <c r="I17" s="4" t="s">
@@ -6623,52 +6712,52 @@
       </c>
       <c r="J17" s="22">
         <f>+(F17+F15)/F13</f>
-        <v>73.648747501032602</v>
+        <v>613.61922066451154</v>
       </c>
       <c r="K17" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="L17" s="47">
+      <c r="L17" s="46">
         <f>2.5*10000/(LN($J$17/8.23))</f>
-        <v>11407.601665013046</v>
-      </c>
-      <c r="M17" s="48">
+        <v>5798.326917374724</v>
+      </c>
+      <c r="M17" s="47">
         <f>10860/(LOG(J17)-0.81)</f>
-        <v>10272.754249049563</v>
-      </c>
-      <c r="N17" s="48">
+        <v>5490.6748263931104</v>
+      </c>
+      <c r="N17" s="47">
         <f>10697.5/(LOG(J17)-0.888527)</f>
-        <v>10931.004115036436</v>
-      </c>
-      <c r="O17" s="47">
+        <v>5632.124857504793</v>
+      </c>
+      <c r="O17" s="46">
         <f>2.5*10000/(LN($J$17/6.91))</f>
-        <v>10564.849693563523</v>
+        <v>5572.3904452448896</v>
       </c>
       <c r="Q17" s="18"/>
       <c r="R17" s="18"/>
       <c r="S17" s="28"/>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B18" s="19">
         <v>6716.5</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="49" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="21">
-        <v>3.9</v>
+        <v>38.78</v>
       </c>
       <c r="E18" s="22">
         <f t="shared" si="0"/>
-        <v>7.208872458410351</v>
+        <v>8.0203507610853748</v>
       </c>
       <c r="F18" s="23">
         <f t="shared" si="1"/>
-        <v>6.5256425307509049</v>
+        <v>3.7794592059412517</v>
       </c>
       <c r="G18" s="24">
         <f t="shared" si="2"/>
-        <v>10.469925749684403</v>
+        <v>112.20895170604055</v>
       </c>
       <c r="H18" s="25"/>
       <c r="I18" s="29"/>
@@ -6680,27 +6769,27 @@
       <c r="R18" s="18"/>
       <c r="S18" s="28"/>
     </row>
-    <row r="19" spans="2:19" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="B19" s="19">
         <v>6730.7</v>
       </c>
-      <c r="C19" s="50" t="s">
+      <c r="C19" s="49" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="21">
-        <v>6.1</v>
+        <v>69.05</v>
       </c>
       <c r="E19" s="22">
         <f t="shared" si="0"/>
-        <v>11.275415896487983</v>
+        <v>14.280691594970218</v>
       </c>
       <c r="F19" s="23">
-        <f t="shared" si="1"/>
-        <v>10.200945599482825</v>
+        <f>+E19*10^(J$11*((2.5634*(B19/10000)^2-4.873*(B19/10000)+1.7636)))</f>
+        <v>6.7005585987165004</v>
       </c>
       <c r="G19" s="24">
-        <f t="shared" si="2"/>
-        <v>10.533046044865021</v>
+        <f>+(E19-F19)/F19*100</f>
+        <v>113.12688165589211</v>
       </c>
       <c r="H19" s="25"/>
       <c r="I19" s="4" t="s">
@@ -6708,288 +6797,277 @@
       </c>
       <c r="J19" s="26">
         <f>+F18/F19</f>
-        <v>0.63970957075604307</v>
+        <v>0.56405136232451003</v>
       </c>
       <c r="K19" s="36" t="s">
         <v>28</v>
       </c>
       <c r="L19" s="37">
         <f>100*SQRT(L17)*(J19-1.49)/(5.62-12.8*J19)</f>
-        <v>3536.0766560122661</v>
+        <v>4407.1411616721189</v>
       </c>
       <c r="M19" s="29"/>
       <c r="Q19" s="18"/>
       <c r="R19" s="18"/>
       <c r="S19" s="28"/>
     </row>
-    <row r="20" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L20" s="69" t="s">
+    <row r="20" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L20" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="M20" s="70" t="s">
+      <c r="M20" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="O20" s="70" t="s">
+      <c r="O20" s="67" t="s">
         <v>82</v>
       </c>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="2:19" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="B21" s="100" t="s">
+    <row r="21" spans="2:19" ht="18" x14ac:dyDescent="0.4">
+      <c r="B21" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="101"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="102"/>
-      <c r="F21" s="102"/>
-      <c r="G21" s="103"/>
-      <c r="K21" s="58" t="s">
+      <c r="C21" s="95"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="96"/>
+      <c r="F21" s="96"/>
+      <c r="G21" s="97"/>
+      <c r="K21" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="L21" s="73">
+      <c r="L21" s="70">
         <f>+L15/L17</f>
-        <v>1.1203855744191122</v>
-      </c>
-      <c r="M21" s="73">
+        <v>127.43895533634048</v>
+      </c>
+      <c r="M21" s="70">
         <f>+N15/M17</f>
-        <v>1.2275738465945059</v>
-      </c>
-      <c r="N21" s="62"/>
-      <c r="O21" s="73">
+        <v>69.514693964973048</v>
+      </c>
+      <c r="N21" s="59"/>
+      <c r="O21" s="70">
         <f>+O15/O17</f>
-        <v>1.2346019092878415</v>
-      </c>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="104" t="s">
+        <v>-811.46978046189122</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B22" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="101" t="s">
+      <c r="C22" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="102"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="102"/>
-      <c r="G22" s="105"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="96"/>
+      <c r="G22" s="99"/>
       <c r="J22" s="40"/>
       <c r="K22" s="40"/>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="57" t="s">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B23" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="53" t="s">
+      <c r="C23" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="56"/>
-      <c r="I23" s="74" t="s">
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="54"/>
+      <c r="I23" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="J23" s="64"/>
-      <c r="L23" s="76" t="s">
+      <c r="J23" s="61"/>
+      <c r="L23" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="M23" s="71" t="s">
+      <c r="M23" s="68" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="54">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B24" s="53">
         <v>3</v>
       </c>
-      <c r="C24" s="53" t="s">
+      <c r="C24" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="56"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="54"/>
       <c r="H24" s="41"/>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="57" t="s">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B25" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="53" t="s">
+      <c r="C25" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="56"/>
-      <c r="I25" s="63" t="s">
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="54"/>
+      <c r="I25" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="J25" s="64"/>
-      <c r="K25" s="65">
+      <c r="J25" s="61"/>
+      <c r="K25" s="62">
         <f>IF(F9&gt;1,LOG((F12+F11)/F9),(F12+F11)/F10)</f>
-        <v>1.6352789261484681</v>
-      </c>
-      <c r="L25" s="61">
+        <v>3.7205755000970426</v>
+      </c>
+      <c r="L25" s="58">
         <f>IF(F9&gt;1,VLOOKUP(K25,Feuil3!U7:V15,2,TRUE),VLOOKUP(K25,Feuil3!U3:V5,2))</f>
+        <v>1</v>
+      </c>
+      <c r="M25" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="N25" s="76" t="str">
+        <f>CONCATENATE(VLOOKUP(L25,Feuil3!X3:Y14,2)," excitation")</f>
+        <v>low excitation</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B26" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="54"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="69"/>
+    </row>
+    <row r="27" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="53">
         <v>9</v>
       </c>
-      <c r="M25" s="66" t="s">
-        <v>52</v>
-      </c>
-      <c r="N25" s="81" t="str">
-        <f>CONCATENATE(VLOOKUP(L25,Feuil3!X3:Y14,2)," excitation")</f>
-        <v>high excitation</v>
-      </c>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="56"/>
-      <c r="K26" s="68"/>
-      <c r="L26" s="60"/>
-      <c r="M26" s="72"/>
-    </row>
-    <row r="27" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="54">
-        <v>9</v>
-      </c>
-      <c r="C27" s="53" t="s">
+      <c r="C27" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="55"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="56"/>
+      <c r="D27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="54"/>
       <c r="H27" s="25"/>
-      <c r="I27" s="63" t="s">
+      <c r="I27" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="J27" s="77">
+      <c r="J27" s="74">
         <v>11</v>
       </c>
-      <c r="K27" s="65">
+      <c r="K27" s="62" t="b">
         <f>+IF($F$9&gt;1,5.54*($F$9/$F$10+0.78))</f>
-        <v>6.041644775485504</v>
-      </c>
-      <c r="L27" s="67">
+        <v>0</v>
+      </c>
+      <c r="L27" s="64">
         <f>+INT(K27)</f>
-        <v>6</v>
-      </c>
-      <c r="M27" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="M27" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="N27" s="94">
+      <c r="N27" s="89">
         <f>10^(4.489+0.1124*K27-0.00172*K27^2)</f>
-        <v>127437.82234013747</v>
-      </c>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="78">
+        <v>30831.879502493568</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B28" s="53">
         <v>10</v>
       </c>
-      <c r="C28" s="79" t="s">
+      <c r="C28" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="80"/>
-      <c r="N28" s="110" t="s">
+      <c r="G28" s="75"/>
+      <c r="N28" s="104" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="78">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B29" s="53">
         <v>11</v>
       </c>
-      <c r="C29" s="53" t="s">
+      <c r="C29" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="80"/>
-      <c r="I29" s="63" t="s">
+      <c r="G29" s="75"/>
+      <c r="I29" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="J29" s="77">
+      <c r="J29" s="74">
         <v>12</v>
       </c>
-      <c r="K29" s="65">
+      <c r="K29" s="62" t="b">
         <f>+IF($F$9&gt;1,5.54*(F9/F10+LOG((F11+F12)/F10)))</f>
-        <v>7.9662956114738126</v>
-      </c>
-      <c r="L29" s="67">
+        <v>0</v>
+      </c>
+      <c r="L29" s="64">
         <f>+INT(K29)</f>
-        <v>7</v>
-      </c>
-      <c r="M29" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="M29" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="N29" s="97">
+      <c r="N29" s="91">
         <f>10^(4.439+0.1174*K29-0.00172*K29^2)</f>
-        <v>184114.79794617722</v>
-      </c>
-    </row>
-    <row r="30" spans="2:19" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="78">
+        <v>27478.941531024004</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" ht="2.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="53">
         <v>12</v>
       </c>
-      <c r="C30" s="96"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="80"/>
+      <c r="G30" s="75"/>
       <c r="H30" s="25"/>
-      <c r="N30" s="98"/>
-    </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="106">
+      <c r="N30" s="92"/>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B31" s="100">
         <v>12</v>
       </c>
-      <c r="C31" s="107" t="s">
+      <c r="C31" s="101" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="108"/>
-      <c r="E31" s="108"/>
-      <c r="F31" s="108"/>
-      <c r="G31" s="109"/>
-      <c r="N31" s="95">
+      <c r="D31" s="102"/>
+      <c r="E31" s="102"/>
+      <c r="F31" s="102"/>
+      <c r="G31" s="103"/>
+      <c r="N31" s="90">
         <f>10^(4.905+1.011162*0.01*F9-1.10692*0.0001*F9^2+6.20572*0.0000001*F9^3)</f>
-        <v>135166.82519765678</v>
-      </c>
-      <c r="O31" s="99" t="s">
+        <v>80352.612218561815</v>
+      </c>
+      <c r="O31" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="Q31" s="70" t="str">
+      <c r="Q31" s="67" t="str">
         <f>+I25</f>
         <v>Gurzadyan 1998             10</v>
       </c>
-      <c r="R31" s="70" t="str">
+      <c r="R31" s="67" t="str">
         <f>+I27</f>
         <v>Dopita 1990</v>
       </c>
-      <c r="S31" s="70" t="s">
+      <c r="S31" s="67" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E32" s="44"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="E32" s="43"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E34" s="38"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E35" s="38"/>
     </row>
   </sheetData>
-  <sortState ref="U29:V37">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="U29:V37">
     <sortCondition ref="U34:U42"/>
   </sortState>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
@@ -6999,22 +7077,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="1.875" customWidth="1"/>
+    <col min="4" max="4" width="1.8984375" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="11.625" customWidth="1"/>
+    <col min="9" max="9" width="11.59765625" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E2" s="4" t="s">
         <v>29</v>
       </c>
@@ -7031,14 +7109,14 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="19">
         <v>4340.47</v>
       </c>
@@ -7047,7 +7125,7 @@
       </c>
       <c r="E4" s="23">
         <f>+Feuil1!F7</f>
-        <v>45.462450010559465</v>
+        <v>60.799645518314634</v>
       </c>
       <c r="F4" s="4">
         <v>46</v>
@@ -7062,7 +7140,7 @@
         <v>47.333333333333336</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="19">
         <v>4363.21</v>
       </c>
@@ -7071,7 +7149,7 @@
       </c>
       <c r="E5" s="23">
         <f>+Feuil1!F8</f>
-        <v>13.404989914636737</v>
+        <v>58.910045440104589</v>
       </c>
       <c r="F5" s="4">
         <v>14</v>
@@ -7086,7 +7164,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="19">
         <v>4685.68</v>
       </c>
@@ -7095,7 +7173,7 @@
       </c>
       <c r="E6" s="23">
         <f>+Feuil1!F9</f>
-        <v>31.059078971726535</v>
+        <v>0</v>
       </c>
       <c r="F6" s="4">
         <v>38</v>
@@ -7110,7 +7188,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="19">
         <v>5006.8500000000004</v>
       </c>
@@ -7119,7 +7197,7 @@
       </c>
       <c r="E7" s="23">
         <f>+Feuil1!F12</f>
-        <v>1012.346047861558</v>
+        <v>278.48748523886042</v>
       </c>
       <c r="F7" s="4">
         <v>950</v>
@@ -7134,7 +7212,7 @@
         <v>1136.6666666666667</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="19">
         <v>5754.57</v>
       </c>
@@ -7143,7 +7221,7 @@
       </c>
       <c r="E8" s="23">
         <f>+Feuil1!F13</f>
-        <v>1.4008855059632634</v>
+        <v>0.54423117572891466</v>
       </c>
       <c r="F8" s="4">
         <v>2</v>
@@ -7158,7 +7236,7 @@
         <v>1.7033333333333334</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="33">
         <v>5875.65</v>
       </c>
@@ -7167,7 +7245,7 @@
       </c>
       <c r="E9" s="23">
         <f>+Feuil1!F14</f>
-        <v>10.438970970086348</v>
+        <v>11.533422560523382</v>
       </c>
       <c r="F9" s="4">
         <v>6.8</v>
@@ -7182,7 +7260,7 @@
         <v>7.3500000000000005</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="19">
         <v>6562.82</v>
       </c>
@@ -7191,7 +7269,7 @@
       </c>
       <c r="E10" s="23">
         <f>+Feuil1!F16</f>
-        <v>282.22697945278031</v>
+        <v>279.25952985408833</v>
       </c>
       <c r="F10" s="4">
         <v>275</v>
@@ -7206,7 +7284,7 @@
         <v>284.33333333333331</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="19">
         <v>6583.39</v>
       </c>
@@ -7215,7 +7293,7 @@
       </c>
       <c r="E11" s="23">
         <f>+Feuil1!F17</f>
-        <v>77.561577438453085</v>
+        <v>51.264270859689816</v>
       </c>
       <c r="F11" s="4">
         <v>95</v>
@@ -7230,7 +7308,7 @@
         <v>91.833333333333329</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="19">
         <v>6716.5</v>
       </c>
@@ -7239,7 +7317,7 @@
       </c>
       <c r="E12" s="23">
         <f>+Feuil1!F18</f>
-        <v>6.5256425307509049</v>
+        <v>3.7794592059412517</v>
       </c>
       <c r="F12" s="4">
         <v>8</v>
@@ -7254,7 +7332,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="19">
         <v>6730.7</v>
       </c>
@@ -7263,7 +7341,7 @@
       </c>
       <c r="E13" s="23">
         <f>+Feuil1!F19</f>
-        <v>10.200945599482825</v>
+        <v>6.7005585987165004</v>
       </c>
       <c r="F13" s="4">
         <v>10</v>
@@ -7278,18 +7356,18 @@
         <v>8.5666666666666664</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>36</v>
       </c>
@@ -7300,32 +7378,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:AJ145"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="25" customWidth="1"/>
-    <col min="3" max="3" width="1.75" customWidth="1"/>
-    <col min="4" max="4" width="6.25" customWidth="1"/>
-    <col min="5" max="5" width="7.375" customWidth="1"/>
-    <col min="6" max="6" width="0.875" customWidth="1"/>
+    <col min="3" max="3" width="1.69921875" customWidth="1"/>
+    <col min="4" max="4" width="6.19921875" customWidth="1"/>
+    <col min="5" max="5" width="7.3984375" customWidth="1"/>
+    <col min="6" max="6" width="0.8984375" customWidth="1"/>
     <col min="7" max="9" width="6" customWidth="1"/>
-    <col min="10" max="10" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="5.8984375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.8984375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
     <col min="27" max="27" width="6" customWidth="1"/>
-    <col min="28" max="36" width="5.625" customWidth="1"/>
+    <col min="28" max="36" width="5.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:36" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" ht="18" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -7344,13 +7422,13 @@
       <c r="J2" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" s="86" t="s">
+      <c r="AB2" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="AC2" s="83"/>
-      <c r="AD2" s="83"/>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="78"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="E3" s="25"/>
       <c r="H3" s="42"/>
       <c r="I3" s="42"/>
@@ -7378,26 +7456,26 @@
       <c r="Y3" t="s">
         <v>59</v>
       </c>
-      <c r="AA3" s="84" t="s">
+      <c r="AA3" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="AB3" s="85" t="s">
+      <c r="AB3" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="AC3" s="85" t="s">
+      <c r="AC3" s="80" t="s">
         <v>70</v>
       </c>
-      <c r="AD3" s="85" t="s">
+      <c r="AD3" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="AE3" s="82"/>
+      <c r="AE3" s="77"/>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="U4">
         <v>7.5</v>
       </c>
@@ -7410,16 +7488,16 @@
       <c r="Y4" t="s">
         <v>59</v>
       </c>
-      <c r="AA4" s="84" t="s">
+      <c r="AA4" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="AB4" s="76">
+      <c r="AB4" s="73">
         <v>1</v>
       </c>
-      <c r="AC4" s="76">
+      <c r="AC4" s="73">
         <v>2</v>
       </c>
-      <c r="AD4" s="76">
+      <c r="AD4" s="73">
         <v>3</v>
       </c>
       <c r="AE4" s="1"/>
@@ -7429,7 +7507,7 @@
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6000</v>
       </c>
@@ -7485,7 +7563,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6100</v>
       </c>
@@ -7534,21 +7612,21 @@
       <c r="Y6" t="s">
         <v>61</v>
       </c>
-      <c r="AB6" s="87" t="s">
+      <c r="AB6" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="AC6" s="88"/>
-      <c r="AD6" s="88"/>
-      <c r="AE6" s="88"/>
-      <c r="AF6" s="89"/>
-      <c r="AG6" s="89" t="s">
+      <c r="AC6" s="83"/>
+      <c r="AD6" s="83"/>
+      <c r="AE6" s="83"/>
+      <c r="AF6" s="84"/>
+      <c r="AG6" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="AH6" s="89"/>
-      <c r="AI6" s="89"/>
-      <c r="AJ6" s="89"/>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AH6" s="84"/>
+      <c r="AI6" s="84"/>
+      <c r="AJ6" s="84"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6200</v>
       </c>
@@ -7603,38 +7681,38 @@
       <c r="Y7" t="s">
         <v>61</v>
       </c>
-      <c r="AA7" s="84" t="s">
+      <c r="AA7" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="AB7" s="76">
+      <c r="AB7" s="73">
         <v>2.7</v>
       </c>
-      <c r="AC7" s="76">
+      <c r="AC7" s="73">
         <v>2.5</v>
       </c>
-      <c r="AD7" s="76">
+      <c r="AD7" s="73">
         <v>2.2999999999999998</v>
       </c>
-      <c r="AE7" s="76">
+      <c r="AE7" s="73">
         <v>2.1</v>
       </c>
-      <c r="AF7" s="76">
+      <c r="AF7" s="73">
         <v>1.9</v>
       </c>
-      <c r="AG7" s="76">
+      <c r="AG7" s="73">
         <v>1.7</v>
       </c>
-      <c r="AH7" s="76">
+      <c r="AH7" s="73">
         <v>1.5</v>
       </c>
-      <c r="AI7" s="76">
+      <c r="AI7" s="73">
         <v>1.2</v>
       </c>
-      <c r="AJ7" s="76">
+      <c r="AJ7" s="73">
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6300</v>
       </c>
@@ -7689,38 +7767,38 @@
       <c r="Y8" t="s">
         <v>61</v>
       </c>
-      <c r="AA8" s="84" t="s">
+      <c r="AA8" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="AB8" s="76">
+      <c r="AB8" s="73">
         <v>4</v>
       </c>
-      <c r="AC8" s="76">
+      <c r="AC8" s="73">
         <v>5</v>
       </c>
-      <c r="AD8" s="76">
+      <c r="AD8" s="73">
         <v>6</v>
       </c>
-      <c r="AE8" s="76">
+      <c r="AE8" s="73">
         <v>7</v>
       </c>
-      <c r="AF8" s="76">
+      <c r="AF8" s="73">
         <v>8</v>
       </c>
-      <c r="AG8" s="76">
+      <c r="AG8" s="73">
         <v>9</v>
       </c>
-      <c r="AH8" s="76">
+      <c r="AH8" s="73">
         <v>10</v>
       </c>
-      <c r="AI8" s="76">
+      <c r="AI8" s="73">
         <v>11</v>
       </c>
-      <c r="AJ8" s="76">
+      <c r="AJ8" s="73">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6400</v>
       </c>
@@ -7776,7 +7854,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6500</v>
       </c>
@@ -7832,7 +7910,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6600</v>
       </c>
@@ -7888,7 +7966,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6700</v>
       </c>
@@ -7944,7 +8022,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6800</v>
       </c>
@@ -8000,7 +8078,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6900</v>
       </c>
@@ -8056,7 +8134,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7000</v>
       </c>
@@ -8106,7 +8184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>7100</v>
       </c>
@@ -8150,7 +8228,7 @@
         <v>1.3824785027898772</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>7200</v>
       </c>
@@ -8194,7 +8272,7 @@
         <v>1.3581310518102321</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>7300</v>
       </c>
@@ -8238,7 +8316,7 @@
         <v>1.3292097443336905</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>7400</v>
       </c>
@@ -8282,7 +8360,7 @@
         <v>1.2952889532592902</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>7500</v>
       </c>
@@ -8326,7 +8404,7 @@
         <v>1.256092107257903</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>7600</v>
       </c>
@@ -8370,7 +8448,7 @@
         <v>1.2115698966433095</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>7700</v>
       </c>
@@ -8414,7 +8492,7 @@
         <v>1.1619747581040687</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>7800</v>
       </c>
@@ -8458,7 +8536,7 @@
         <v>1.1079137226876594</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>7900</v>
       </c>
@@ -8502,7 +8580,7 @@
         <v>1.0503598666915717</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8000</v>
       </c>
@@ -8546,7 +8624,7 @@
         <v>0.99060751723968976</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>8100</v>
       </c>
@@ -8590,7 +8668,7 @@
         <v>0.93016887554994498</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>8200</v>
       </c>
@@ -8634,7 +8712,7 @@
         <v>0.87062662785879286</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>8300</v>
       </c>
@@ -8678,7 +8756,7 @@
         <v>0.81347163206606055</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>8400</v>
       </c>
@@ -8722,7 +8800,7 @@
         <v>0.75995998320732228</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>8500</v>
       </c>
@@ -8766,7 +8844,7 @@
         <v>0.71101701636354875</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>8600</v>
       </c>
@@ -8810,7 +8888,7 @@
         <v>0.66720052144458186</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>8700</v>
       </c>
@@ -8854,7 +8932,7 @@
         <v>0.62871878715264418</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>8800</v>
       </c>
@@ -8898,7 +8976,7 @@
         <v>0.59548750958542274</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>8900</v>
       </c>
@@ -8942,7 +9020,7 @@
         <v>0.56720571523565144</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>9000</v>
       </c>
@@ -8986,7 +9064,7 @@
         <v>0.5434333861694346</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>9100</v>
       </c>
@@ -9030,7 +9108,7 @@
         <v>0.52365926810115837</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>9200</v>
       </c>
@@ -9074,7 +9152,7 @@
         <v>0.50735342400376504</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>9300</v>
       </c>
@@ -9118,7 +9196,7 @@
         <v>0.49400374866789803</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>9400</v>
       </c>
@@ -9162,7 +9240,7 @@
         <v>0.48313841342580671</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>9500</v>
       </c>
@@ -9206,7 +9284,7 @@
         <v>0.47433735494606022</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>9600</v>
       </c>
@@ -9250,7 +9328,7 @@
         <v>0.46723601074993065</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>9700</v>
       </c>
@@ -9294,7 +9372,7 @@
         <v>0.46152404987797202</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>9800</v>
       </c>
@@ -9338,7 +9416,7 @@
         <v>0.45694120841866892</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>9900</v>
       </c>
@@ -9382,7 +9460,7 @@
         <v>0.45327171900948759</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>10000</v>
       </c>
@@ -9426,7 +9504,7 @@
         <v>0.45033830986305806</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>10100</v>
       </c>
@@ -9470,7 +9548,7 @@
         <v>0.44799636357442774</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10200</v>
       </c>
@@ -9514,7 +9592,7 @@
         <v>0.44612855697235337</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>10300</v>
       </c>
@@ -9558,7 +9636,7 @@
         <v>0.44464012669068831</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>10400</v>
       </c>
@@ -9602,7 +9680,7 @@
         <v>0.4434547961567159</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>10500</v>
       </c>
@@ -9646,7 +9724,7 @@
         <v>0.44251133727424247</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>10600</v>
       </c>
@@ -9690,7 +9768,7 @@
         <v>0.44176070813342694</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>10700</v>
       </c>
@@ -9734,7 +9812,7 @@
         <v>0.44116369511537473</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>10800</v>
       </c>
@@ -9778,7 +9856,7 @@
         <v>0.44068898597067141</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>10900</v>
       </c>
@@ -9822,7 +9900,7 @@
         <v>0.44031160475246001</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>11000</v>
       </c>
@@ -9866,7 +9944,7 @@
         <v>0.43899774947321485</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>11100</v>
       </c>
@@ -9910,7 +9988,7 @@
         <v>0.43886618302731767</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>11200</v>
       </c>
@@ -9954,7 +10032,7 @@
         <v>0.43885302457103437</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>11300</v>
       </c>
@@ -9998,7 +10076,7 @@
         <v>0.43885170870728646</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>11400</v>
       </c>
@@ -10042,7 +10120,7 @@
         <v>0.43885157712073047</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>11500</v>
       </c>
@@ -10086,7 +10164,7 @@
         <v>0.43885156396207314</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>11600</v>
       </c>
@@ -10130,7 +10208,7 @@
         <v>0.43885156264620734</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>11700</v>
       </c>
@@ -10174,7 +10252,7 @@
         <v>0.43885156251462082</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>11800</v>
       </c>
@@ -10218,7 +10296,7 @@
         <v>0.43885156250146218</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>11900</v>
       </c>
@@ -10262,7 +10340,7 @@
         <v>0.43885156250014629</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>12000</v>
       </c>
@@ -10306,7 +10384,7 @@
         <v>0.43885156250001461</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>12100</v>
       </c>
@@ -10350,7 +10428,7 @@
         <v>0.43885156250000151</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>12200</v>
       </c>
@@ -10375,7 +10453,7 @@
       </c>
       <c r="I67">
         <f t="shared" si="12"/>
-        <v>1123349762522962.7</v>
+        <v>1123349762522962.8</v>
       </c>
       <c r="J67" s="35">
         <f t="shared" si="13"/>
@@ -10394,7 +10472,7 @@
         <v>0.43885156250000024</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>12300</v>
       </c>
@@ -10438,7 +10516,7 @@
         <v>0.43885156250000001</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>12400</v>
       </c>
@@ -10482,7 +10560,7 @@
         <v>0.43885156250000001</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>12500</v>
       </c>
@@ -10526,7 +10604,7 @@
         <v>0.43885156250000001</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>12600</v>
       </c>
@@ -10570,7 +10648,7 @@
         <v>0.43885156250000001</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>12700</v>
       </c>
@@ -10614,7 +10692,7 @@
         <v>0.43885156250000001</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>12800</v>
       </c>
@@ -10658,7 +10736,7 @@
         <v>0.43885156250000007</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>12900</v>
       </c>
@@ -10675,7 +10753,7 @@
         <v>57.155207777964897</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>13000</v>
       </c>
@@ -10692,7 +10770,7 @@
         <v>56.309481865883583</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>13100</v>
       </c>
@@ -10709,7 +10787,7 @@
         <v>55.488897808418344</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>13200</v>
       </c>
@@ -10726,7 +10804,7 @@
         <v>54.692435469366281</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>13300</v>
       </c>
@@ -10743,7 +10821,7 @@
         <v>53.919126298464533</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>13400</v>
       </c>
@@ -10760,7 +10838,7 @@
         <v>53.168050236754119</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>13500</v>
       </c>
@@ -10777,7 +10855,7 @@
         <v>52.438332835422855</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>13600</v>
       </c>
@@ -10794,7 +10872,7 @@
         <v>51.729142571554917</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>13700</v>
       </c>
@@ -10811,7 +10889,7 @@
         <v>51.0396883456391</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>13800</v>
       </c>
@@ -10828,7 +10906,7 @@
         <v>50.369217146979231</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>13900</v>
       </c>
@@ -10845,7 +10923,7 @@
         <v>49.717011874320448</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>14000</v>
       </c>
@@ -10862,7 +10940,7 @@
         <v>49.082389300067732</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>14100</v>
       </c>
@@ -10879,7 +10957,7 @@
         <v>48.464698167437369</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>14200</v>
       </c>
@@ -10896,7 +10974,7 @@
         <v>47.863317410760196</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>14300</v>
       </c>
@@ -10913,7 +10991,7 @@
         <v>47.277654489952603</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>14400</v>
       </c>
@@ -10930,7 +11008,7 @@
         <v>46.707143830898893</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>14500</v>
       </c>
@@ -10947,7 +11025,7 @@
         <v>46.151245364150654</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>14600</v>
       </c>
@@ -10964,7 +11042,7 @@
         <v>45.609443154952892</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>14700</v>
       </c>
@@ -10981,7 +11059,7 @@
         <v>45.081244118158459</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>14800</v>
       </c>
@@ -10998,7 +11076,7 @@
         <v>44.566176812095939</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>14900</v>
       </c>
@@ -11015,7 +11093,7 @@
         <v>44.063790305916655</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>15000</v>
       </c>
@@ -11032,7 +11110,7 @@
         <v>43.573653115368344</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>15100</v>
       </c>
@@ -11049,7 +11127,7 @@
         <v>43.095352202328087</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>15200</v>
       </c>
@@ -11066,7 +11144,7 @@
         <v>42.628492033781477</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>15300</v>
       </c>
@@ -11083,7 +11161,7 @@
         <v>42.172693696258598</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>15400</v>
       </c>
@@ -11100,7 +11178,7 @@
         <v>41.727594062034818</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>15500</v>
       </c>
@@ -11117,7 +11195,7 @@
         <v>41.292845003678032</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>15600</v>
       </c>
@@ -11134,7 +11212,7 @@
         <v>40.868112653774169</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>15700</v>
       </c>
@@ -11151,7 +11229,7 @@
         <v>40.453076706894109</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>15800</v>
       </c>
@@ -11168,7 +11246,7 @@
         <v>40.04742976107714</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>15900</v>
       </c>
@@ -11185,7 +11263,7 @@
         <v>39.65087669630163</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>16000</v>
       </c>
@@ -11202,7 +11280,7 @@
         <v>39.263134087593372</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>16100</v>
       </c>
@@ -11219,7 +11297,7 @@
         <v>38.883929650588669</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>16200</v>
       </c>
@@ -11236,7 +11314,7 @@
         <v>38.513001717521355</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>16300</v>
       </c>
@@ -11253,7 +11331,7 @@
         <v>38.150098741745346</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>16400</v>
       </c>
@@ -11270,7 +11348,7 @@
         <v>37.794978829033781</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>16500</v>
       </c>
@@ -11287,7 +11365,7 @@
         <v>37.447409294017291</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>16600</v>
       </c>
@@ -11304,7 +11382,7 @@
         <v>37.107166240234747</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>16700</v>
       </c>
@@ -11321,7 +11399,7 @@
         <v>36.774034162373496</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>16800</v>
       </c>
@@ -11338,7 +11416,7 @@
         <v>36.447805569371326</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>16900</v>
       </c>
@@ -11355,7 +11433,7 @@
         <v>36.128280627140967</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>17000</v>
       </c>
@@ -11372,7 +11450,7 @@
         <v>35.815266819759842</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>17100</v>
       </c>
@@ -11389,7 +11467,7 @@
         <v>35.508578628043928</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>17200</v>
       </c>
@@ -11406,7 +11484,7 @@
         <v>35.208037224494902</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>17300</v>
       </c>
@@ -11423,7 +11501,7 @@
         <v>34.913470183675564</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>17400</v>
       </c>
@@ -11440,7 +11518,7 @@
         <v>34.624711207128762</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>17500</v>
       </c>
@@ -11457,7 +11535,7 @@
         <v>34.34159986201233</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>17600</v>
       </c>
@@ -11474,7 +11552,7 @@
         <v>34.063981332674238</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>17700</v>
       </c>
@@ -11491,7 +11569,7 @@
         <v>33.791706184441701</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>17800</v>
       </c>
@@ -11508,7 +11586,7 @@
         <v>33.52463013894306</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>17900</v>
       </c>
@@ -11525,7 +11603,7 @@
         <v>33.262613860323803</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>18000</v>
       </c>
@@ -11542,7 +11620,7 @@
         <v>33.005522751757361</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>18100</v>
       </c>
@@ -11559,7 +11637,7 @@
         <v>32.753226761688261</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>18200</v>
       </c>
@@ -11576,7 +11654,7 @@
         <v>32.505600199279421</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>18300</v>
       </c>
@@ -11593,7 +11671,7 @@
         <v>32.262521558567265</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>18400</v>
       </c>
@@ -11610,7 +11688,7 @@
         <v>32.023873350858395</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>18500</v>
       </c>
@@ -11627,7 +11705,7 @@
         <v>31.78954194492913</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>18600</v>
       </c>
@@ -11644,7 +11722,7 @@
         <v>31.559417414615677</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>18700</v>
       </c>
@@ -11661,7 +11739,7 @@
         <v>31.333393393406524</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>18800</v>
       </c>
@@ -11678,7 +11756,7 @@
         <v>31.111366935671853</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>18900</v>
       </c>
@@ -11695,7 +11773,7 @@
         <v>30.893238384185825</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>19000</v>
       </c>
@@ -11712,7 +11790,7 @@
         <v>30.678911243617499</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>19100</v>
       </c>
@@ -11729,7 +11807,7 @@
         <v>30.468292059684874</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>19200</v>
       </c>
@@ -11746,7 +11824,7 @@
         <v>30.261290303684063</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>19300</v>
       </c>
@@ -11763,7 +11841,7 @@
         <v>30.057818262121724</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>19400</v>
       </c>
@@ -11780,7 +11858,7 @@
         <v>29.857790931194533</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>19500</v>
       </c>
@@ -11797,7 +11875,7 @@
         <v>29.66112591587364</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>19600</v>
       </c>
@@ -11814,7 +11892,7 @@
         <v>29.467743333365686</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>19700</v>
       </c>
@@ -11831,7 +11909,7 @@
         <v>29.277565720734483</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>19800</v>
       </c>
@@ -11848,7 +11926,7 @@
         <v>29.09051794647948</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>19900</v>
       </c>
@@ -11865,7 +11943,7 @@
         <v>28.906527125878299</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>20000</v>
       </c>

</xml_diff>

<commit_message>
added tooltips to headers
</commit_message>
<xml_diff>
--- a/Analyse_NP.xlsx
+++ b/Analyse_NP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GAYRARD\Documents\GitHub\Planetary-Nebula-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097410E6-16C6-4550-BE8B-AE4B07314491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEE2EB6-B78C-4375-81C3-B2DCBFD9437F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4404" yWindow="720" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3852" yWindow="1020" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -6144,8 +6144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:S35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="89" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6282,7 +6282,7 @@
         <v>45.944324950363999</v>
       </c>
       <c r="F7" s="23">
-        <f t="shared" ref="F7:F19" si="1">+E7*10^(J$11*((2.5634*(B7/10000)^2-4.873*(B7/10000)+1.7636)))</f>
+        <f t="shared" ref="F7:F18" si="1">+E7*10^(J$11*((2.5634*(B7/10000)^2-4.873*(B7/10000)+1.7636)))</f>
         <v>60.799645518314634</v>
       </c>
       <c r="G7" s="24">
@@ -6330,7 +6330,7 @@
         <v>58.910045440104589</v>
       </c>
       <c r="G8" s="24">
-        <f t="shared" ref="G8:G19" si="2">+(E8-F8)/F8*100</f>
+        <f t="shared" ref="G8:G18" si="2">+(E8-F8)/F8*100</f>
         <v>-23.459281461053656</v>
       </c>
       <c r="H8" s="25"/>

</xml_diff>